<commit_message>
skibidi bop mmmm dada
</commit_message>
<xml_diff>
--- a/Customer Database.xlsx
+++ b/Customer Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ps-fbzznf3\Lab\Lab recovery\Recreational Water\Final Reports\BacReportWebsite\BacteriologicalReports.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D6D07C-1F35-4544-B172-F4B53315C3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A272A496-56F8-4B15-9631-E5AC1E0D0028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3566" uniqueCount="3291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3569" uniqueCount="3293">
   <si>
     <t>C-VI096</t>
   </si>
@@ -9909,13 +9909,19 @@
   </si>
   <si>
     <t>C-RI195</t>
+  </si>
+  <si>
+    <t>C-CO140</t>
+  </si>
+  <si>
+    <t>Comfort Inn -  Connellsville</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9939,6 +9945,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -9980,7 +9991,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -9995,7 +10006,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10301,8 +10317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1402"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1361" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B1402" sqref="B1402"/>
+    <sheetView tabSelected="1" topLeftCell="A1369" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A1409" sqref="A1409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23792,7 +23808,7 @@
       </c>
     </row>
     <row r="1391" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1391" s="8" t="s">
+      <c r="A1391" t="s">
         <v>3290</v>
       </c>
       <c r="B1391" s="6">
@@ -23883,8 +23899,22 @@
         <v>3289</v>
       </c>
     </row>
-    <row r="1401" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1402" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1401" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1401" s="4" t="s">
+        <v>3291</v>
+      </c>
+      <c r="B1401" s="9">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1402" s="8" t="s">
+        <v>3292</v>
+      </c>
+      <c r="B1402" s="4" t="s">
+        <v>554</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated Customer Database after rollback
</commit_message>
<xml_diff>
--- a/Customer Database.xlsx
+++ b/Customer Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ps-fbzznf3\Lab\Lab recovery\Recreational Water\Final Reports\BacReportWebsite\BacteriologicalReports.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A272A496-56F8-4B15-9631-E5AC1E0D0028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E032EDC4-ADE5-4804-9379-C22253062382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DavidSheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3569" uniqueCount="3293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3577" uniqueCount="3299">
   <si>
     <t>C-VI096</t>
   </si>
@@ -9915,6 +9915,24 @@
   </si>
   <si>
     <t>Comfort Inn -  Connellsville</t>
+  </si>
+  <si>
+    <t>T-AQ110</t>
+  </si>
+  <si>
+    <t>Aqua Pools</t>
+  </si>
+  <si>
+    <t>Pool</t>
+  </si>
+  <si>
+    <t>Spa</t>
+  </si>
+  <si>
+    <t>T-SP130</t>
+  </si>
+  <si>
+    <t>Specialty Pools</t>
   </si>
 </sst>
 </file>
@@ -9991,7 +10009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -10010,6 +10028,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -10315,10 +10336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P1402"/>
+  <dimension ref="A1:P1406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1369" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A1409" sqref="A1409"/>
+    <sheetView tabSelected="1" topLeftCell="A1378" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C1400" sqref="C1400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23915,6 +23936,50 @@
         <v>554</v>
       </c>
     </row>
+    <row r="1403" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1403" t="s">
+        <v>3293</v>
+      </c>
+      <c r="B1403" s="10">
+        <v>5000</v>
+      </c>
+      <c r="C1403" s="10">
+        <v>5001</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1404" t="s">
+        <v>3294</v>
+      </c>
+      <c r="B1404" t="s">
+        <v>3295</v>
+      </c>
+      <c r="C1404" t="s">
+        <v>3296</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1405" s="4" t="s">
+        <v>3297</v>
+      </c>
+      <c r="B1405" s="9">
+        <v>5010</v>
+      </c>
+      <c r="C1405" s="9">
+        <v>5011</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1406" s="4" t="s">
+        <v>3298</v>
+      </c>
+      <c r="B1406" s="4" t="s">
+        <v>3295</v>
+      </c>
+      <c r="C1406" s="4" t="s">
+        <v>3296</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>